<commit_message>
#3 Updated todo history test case documentation
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - ToDoHistory.xlsx
+++ b/TestCases/Test Cases - ToDoHistory.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral\Desktop\ETI CA1.2\To be committed\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral\Desktop\ETI CA1.2\ETIToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53F10E28-5FC7-4B99-ACFA-2F831A65A540}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DFF877-D215-4807-9742-75BE312E7C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -76,6 +76,15 @@
   </si>
   <si>
     <t>The user will be able to see the archived item from to-do page on the to-do history page.</t>
+  </si>
+  <si>
+    <t>Test deleted to-do item is showing in to-do history page</t>
+  </si>
+  <si>
+    <t>To test if the to-do item is still showing in the to-do history page after the item is deleted from the to-do page.</t>
+  </si>
+  <si>
+    <t>The user will be able to see the deleted item in the to-do history page.</t>
   </si>
 </sst>
 </file>
@@ -451,8 +460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -537,13 +546,27 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
+      <c r="A4" s="8">
+        <v>3.2</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="5"/>

</xml_diff>

<commit_message>
#24 Tested and updated test outputs picture and test cases documentation
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - ToDoHistory.xlsx
+++ b/TestCases/Test Cases - ToDoHistory.xlsx
@@ -5,17 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral\Desktop\ETI CA1.2\ETIToDoList\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\new etitodolist\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8DFF877-D215-4807-9742-75BE312E7C64}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9594872E-8CC2-4E09-8226-F21A10920554}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="19">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -51,9 +51,6 @@
     <t>Fail/Pass</t>
   </si>
   <si>
-    <t>Fail</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
@@ -85,6 +82,12 @@
   </si>
   <si>
     <t>The user will be able to see the deleted item in the to-do history page.</t>
+  </si>
+  <si>
+    <t>Same as expected outcome.</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -460,8 +463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -478,7 +481,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -504,22 +507,22 @@
         <v>3</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="D2" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="8" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -527,22 +530,22 @@
         <v>3.1</v>
       </c>
       <c r="B3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>6</v>
+      <c r="F3" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
@@ -550,22 +553,22 @@
         <v>3.2</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="D4" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="8" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>7</v>
-      </c>
       <c r="G4" s="8" t="s">
-        <v>6</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
#35 Updated todo history test case documentation with new test case to filter todo history by user
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - ToDoHistory.xlsx
+++ b/TestCases/Test Cases - ToDoHistory.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Desktop\IT2017\Yr 3 Sem 2\ETI\test master 5\ETI_ToDoList\TestCases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B834EDD0-298D-486E-957D-3577EED8A10C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74E02E9-A5C0-464E-982C-51CA3327C32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -91,6 +91,18 @@
   </si>
   <si>
     <t>Justifications (if any)</t>
+  </si>
+  <si>
+    <t>Fail</t>
+  </si>
+  <si>
+    <t>Test displaying of individual to-do history for each user</t>
+  </si>
+  <si>
+    <t>To test if the to-do history shown are the ones created by the user and not other users.</t>
+  </si>
+  <si>
+    <t>After user log in, he/she sees only his/her own to-do history. Logging into another user's account will show a different list of to-do history.</t>
   </si>
 </sst>
 </file>
@@ -466,8 +478,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -587,13 +599,30 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="5"/>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
+      <c r="A5" s="8">
+        <v>3.3</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="6" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5"/>

</xml_diff>

<commit_message>
#37 Update test case documentation and test_cases_output_todohistory picture
Tested and working. Updated test case documentation and test output accordingly.
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - ToDoHistory.xlsx
+++ b/TestCases/Test Cases - ToDoHistory.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral\Desktop\ETI Todolist testing #37\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B74E02E9-A5C0-464E-982C-51CA3327C32F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A28872-E7C3-4173-A439-93FAB40D0E75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="23">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>Justifications (if any)</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>Test displaying of individual to-do history for each user</t>
@@ -478,23 +475,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4:G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="3" customWidth="1"/>
-    <col min="6" max="7" width="17.42578125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="4.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" style="3" customWidth="1"/>
+    <col min="4" max="4" width="58.7265625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="27.7265625" style="3" customWidth="1"/>
+    <col min="6" max="7" width="17.453125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="24.54296875" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -520,7 +517,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7">
         <v>3</v>
       </c>
@@ -546,7 +543,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>3.1</v>
       </c>
@@ -572,7 +569,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="8">
         <v>3.2</v>
       </c>
@@ -598,33 +595,33 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="56.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8">
         <v>3.3</v>
       </c>
       <c r="B5" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>21</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>22</v>
       </c>
       <c r="D5" s="8" t="s">
         <v>6</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>6</v>
+        <v>17</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -633,7 +630,7 @@
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
     </row>
-    <row r="7" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="5"/>
       <c r="B7" s="5"/>
       <c r="C7" s="5"/>
@@ -642,7 +639,7 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
     </row>
-    <row r="8" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6"/>
       <c r="B8" s="5"/>
       <c r="C8" s="5"/>
@@ -651,7 +648,7 @@
       <c r="F8" s="5"/>
       <c r="G8" s="5"/>
     </row>
-    <row r="9" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5"/>
       <c r="B9" s="5"/>
       <c r="C9" s="5"/>
@@ -660,7 +657,7 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
     </row>
-    <row r="10" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="5"/>
       <c r="B10" s="5"/>
       <c r="C10" s="5"/>
@@ -669,7 +666,7 @@
       <c r="F10" s="5"/>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="5"/>
       <c r="B11" s="5"/>
       <c r="C11" s="5"/>
@@ -678,7 +675,7 @@
       <c r="F11" s="5"/>
       <c r="G11" s="5"/>
     </row>
-    <row r="12" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="6"/>
       <c r="B12" s="5"/>
       <c r="C12" s="5"/>
@@ -687,7 +684,7 @@
       <c r="F12" s="5"/>
       <c r="G12" s="5"/>
     </row>
-    <row r="13" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="5"/>
@@ -696,7 +693,7 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
     </row>
-    <row r="14" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="5"/>
@@ -705,7 +702,7 @@
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
     </row>
-    <row r="15" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" ht="35.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>